<commit_message>
update source to capture and show output v2
</commit_message>
<xml_diff>
--- a/Image2Gcode/excel/time_processing.xlsx
+++ b/Image2Gcode/excel/time_processing.xlsx
@@ -522,11 +522,11 @@
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="n">
-        <v>1.98</v>
+        <v>2.091</v>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
-        <v>801</v>
+        <v>741</v>
       </c>
     </row>
     <row r="3">
@@ -534,7 +534,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>TỔNG: 1.980 giây</t>
+          <t>TỔNG: 2.091 giây</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>

</xml_diff>

<commit_message>
update source for capture & show output v3
</commit_message>
<xml_diff>
--- a/Image2Gcode/excel/time_processing.xlsx
+++ b/Image2Gcode/excel/time_processing.xlsx
@@ -517,16 +517,16 @@
     <row r="2" ht="85" customHeight="1">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1.jpg</t>
+          <t>5.jpg</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="n">
-        <v>2.091</v>
+        <v>1.298</v>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
-        <v>741</v>
+        <v>828</v>
       </c>
     </row>
     <row r="3">
@@ -534,7 +534,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>TỔNG: 2.091 giây</t>
+          <t>TỔNG: 1.298 giây</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>

</xml_diff>

<commit_message>
fix choosing image error and display lag
</commit_message>
<xml_diff>
--- a/Image2Gcode/excel/time_processing.xlsx
+++ b/Image2Gcode/excel/time_processing.xlsx
@@ -522,11 +522,11 @@
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="n">
-        <v>1.288</v>
+        <v>2.015</v>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
-        <v>492</v>
+        <v>552</v>
       </c>
     </row>
     <row r="3">
@@ -534,7 +534,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>TỔNG: 1.288 giây</t>
+          <t>TỔNG: 2.015 giây</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>

</xml_diff>

<commit_message>
update source code for generate gcode
- Intergrate gcode gen for robot
- Add switch camera
- Fix lagging while using image processing and gen gcode
- Add folder simulate

Signed-off-by: Duy Vo <duy.vierobot@gmail.com>
</commit_message>
<xml_diff>
--- a/Image2Gcode/excel/time_processing.xlsx
+++ b/Image2Gcode/excel/time_processing.xlsx
@@ -517,16 +517,16 @@
     <row r="2" ht="85" customHeight="1">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2.jpg</t>
+          <t>1.jpg</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="n">
-        <v>2.015</v>
+        <v>1.454</v>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
-        <v>552</v>
+        <v>380</v>
       </c>
     </row>
     <row r="3">
@@ -534,7 +534,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>TỔNG: 2.015 giây</t>
+          <t>TỔNG: 1.454 giây</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>

</xml_diff>

<commit_message>
add simulate image for UI
</commit_message>
<xml_diff>
--- a/Image2Gcode/excel/time_processing.xlsx
+++ b/Image2Gcode/excel/time_processing.xlsx
@@ -522,11 +522,11 @@
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="n">
-        <v>1.454</v>
+        <v>1.38</v>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
-        <v>380</v>
+        <v>305</v>
       </c>
     </row>
     <row r="3">
@@ -534,7 +534,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>TỔNG: 1.454 giây</t>
+          <t>TỔNG: 1.380 giây</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>

</xml_diff>

<commit_message>
receive data from phone
</commit_message>
<xml_diff>
--- a/Image2Gcode/excel/time_processing.xlsx
+++ b/Image2Gcode/excel/time_processing.xlsx
@@ -517,16 +517,16 @@
     <row r="2" ht="85" customHeight="1">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1.jpg</t>
+          <t>2.jpg</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="n">
-        <v>1.38</v>
+        <v>1.43</v>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
-        <v>305</v>
+        <v>364</v>
       </c>
     </row>
     <row r="3">
@@ -534,7 +534,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>TỔNG: 1.380 giây</t>
+          <t>TỔNG: 1.430 giây</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>

</xml_diff>

<commit_message>
add time respone for recv img from phone
</commit_message>
<xml_diff>
--- a/Image2Gcode/excel/time_processing.xlsx
+++ b/Image2Gcode/excel/time_processing.xlsx
@@ -137,7 +137,7 @@
       <row>1</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="952500" cy="714375"/>
+    <ext cx="533400" cy="952500"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -517,16 +517,16 @@
     <row r="2" ht="85" customHeight="1">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2.jpg</t>
+          <t>1.jpg</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="n">
-        <v>1.43</v>
+        <v>2.395</v>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
-        <v>364</v>
+        <v>437</v>
       </c>
     </row>
     <row r="3">
@@ -534,7 +534,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>TỔNG: 1.430 giây</t>
+          <t>TỔNG: 2.395 giây</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>

</xml_diff>

<commit_message>
add consine, camera, add new reset
</commit_message>
<xml_diff>
--- a/Image2Gcode/excel/time_processing.xlsx
+++ b/Image2Gcode/excel/time_processing.xlsx
@@ -128,61 +128,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>1</col>
-      <colOff>0</colOff>
-      <row>1</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="533400" cy="952500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="1" name="Image 1" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>3</col>
-      <colOff>0</colOff>
-      <row>1</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="952500" cy="952500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="2" name="Image 2" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -472,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,34 +459,18 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="85" customHeight="1">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1.jpg</t>
-        </is>
-      </c>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
       <c r="B2" t="inlineStr"/>
-      <c r="C2" t="n">
-        <v>2.395</v>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>TỔNG: 0.000 giây</t>
+        </is>
       </c>
       <c r="D2" t="inlineStr"/>
-      <c r="E2" t="n">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" s="1" t="inlineStr">
-        <is>
-          <t>TỔNG: 2.395 giây</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>